<commit_message>
latest. update week 4
</commit_message>
<xml_diff>
--- a/Master_comp.xlsx
+++ b/Master_comp.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\612721\1_Projects\Bourbon_Chasers_MASTER\Bourbon_Chasers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5CC1CD9-87DA-4880-8236-35BE8CE3B394}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89C6B6B4-5D5F-48AA-A972-1DE0D404A276}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{1EF4F618-38B6-4D40-964A-FE6EA7248209}"/>
   </bookViews>
@@ -42,9 +42,6 @@
     <t>Week 1 -- May 1 - 8</t>
   </si>
   <si>
-    <t>Week 4</t>
-  </si>
-  <si>
     <t>Week 5</t>
   </si>
   <si>
@@ -97,6 +94,9 @@
   </si>
   <si>
     <t>Week 3 -- May 16 - 22</t>
+  </si>
+  <si>
+    <t>Week 4 -- May 23 - 29</t>
   </si>
 </sst>
 </file>
@@ -472,8 +472,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0652209-7C2F-4DC6-AE94-2767734CF0E0}">
   <dimension ref="A1:K11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="O6" sqref="O6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -481,8 +481,8 @@
     <col min="1" max="1" width="14.26953125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19" bestFit="1" customWidth="1"/>
-    <col min="5" max="10" width="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="19" bestFit="1" customWidth="1"/>
+    <col min="6" max="10" width="7" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -494,36 +494,36 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B2" s="2">
         <v>193.1</v>
@@ -534,8 +534,8 @@
       <c r="D2">
         <v>250.3</v>
       </c>
-      <c r="E2" s="2">
-        <v>0</v>
+      <c r="E2">
+        <v>112.9</v>
       </c>
       <c r="F2" s="2">
         <v>0</v>
@@ -558,7 +558,7 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B3">
         <v>253.6</v>
@@ -570,7 +570,7 @@
         <v>290.2</v>
       </c>
       <c r="E3" s="2">
-        <v>0</v>
+        <v>253.6</v>
       </c>
       <c r="F3" s="2">
         <v>0</v>
@@ -593,7 +593,7 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B4" s="2">
         <v>132.5</v>
@@ -605,7 +605,7 @@
         <v>367.8</v>
       </c>
       <c r="E4" s="2">
-        <v>0</v>
+        <v>48.4</v>
       </c>
       <c r="F4" s="2">
         <v>0</v>
@@ -628,7 +628,7 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B5" s="2">
         <v>107.5</v>
@@ -640,7 +640,7 @@
         <v>282.89999999999998</v>
       </c>
       <c r="E5" s="2">
-        <v>0</v>
+        <v>178.8</v>
       </c>
       <c r="F5" s="2">
         <v>0</v>
@@ -663,7 +663,7 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B6" s="2">
         <v>307.60000000000002</v>
@@ -675,7 +675,7 @@
         <v>346.2</v>
       </c>
       <c r="E6" s="2">
-        <v>0</v>
+        <v>288.8</v>
       </c>
       <c r="F6" s="2">
         <v>0</v>
@@ -698,7 +698,7 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B7" s="2">
         <v>370.6</v>
@@ -710,7 +710,7 @@
         <v>294.3</v>
       </c>
       <c r="E7" s="2">
-        <v>0</v>
+        <v>284.39999999999998</v>
       </c>
       <c r="F7" s="2">
         <v>0</v>
@@ -733,7 +733,7 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B8" s="2">
         <v>25</v>
@@ -745,7 +745,7 @@
         <v>88.5</v>
       </c>
       <c r="E8" s="2">
-        <v>0</v>
+        <v>126.3</v>
       </c>
       <c r="F8" s="2">
         <v>0</v>
@@ -768,7 +768,7 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B9" s="2">
         <v>31</v>
@@ -780,7 +780,7 @@
         <v>320.8</v>
       </c>
       <c r="E9" s="2">
-        <v>0</v>
+        <v>194.2</v>
       </c>
       <c r="F9" s="2">
         <v>0</v>
@@ -803,7 +803,7 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B10" s="2">
         <v>0</v>
@@ -815,7 +815,7 @@
         <v>30</v>
       </c>
       <c r="E10" s="2">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="F10" s="2">
         <v>0</v>
@@ -838,7 +838,7 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B11" s="2">
         <v>497.4</v>
@@ -851,7 +851,7 @@
         <v>89.3</v>
       </c>
       <c r="E11" s="2">
-        <v>0</v>
+        <v>126.9</v>
       </c>
       <c r="F11" s="2">
         <v>0</v>

</xml_diff>

<commit_message>
latest. updated week 5 points
</commit_message>
<xml_diff>
--- a/Master_comp.xlsx
+++ b/Master_comp.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\612721\1_Projects\Bourbon_Chasers_MASTER\Bourbon_Chasers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89C6B6B4-5D5F-48AA-A972-1DE0D404A276}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A179CA80-388D-457C-9F70-B61C989D02D5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{1EF4F618-38B6-4D40-964A-FE6EA7248209}"/>
   </bookViews>
@@ -42,9 +42,6 @@
     <t>Week 1 -- May 1 - 8</t>
   </si>
   <si>
-    <t>Week 5</t>
-  </si>
-  <si>
     <t>Week 6</t>
   </si>
   <si>
@@ -97,6 +94,9 @@
   </si>
   <si>
     <t>Week 4 -- May 23 - 29</t>
+  </si>
+  <si>
+    <t>Week 5 -- May 30 - June 5</t>
   </si>
 </sst>
 </file>
@@ -470,10 +470,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0652209-7C2F-4DC6-AE94-2767734CF0E0}">
-  <dimension ref="A1:K11"/>
+  <dimension ref="A1:K30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -482,7 +482,8 @@
     <col min="2" max="2" width="17" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="19" bestFit="1" customWidth="1"/>
-    <col min="6" max="10" width="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.36328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="10" width="7" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -494,36 +495,36 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B2" s="2">
         <v>193.1</v>
@@ -538,7 +539,7 @@
         <v>112.9</v>
       </c>
       <c r="F2" s="2">
-        <v>0</v>
+        <v>38.6</v>
       </c>
       <c r="G2" s="2">
         <v>0</v>
@@ -558,7 +559,7 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B3">
         <v>253.6</v>
@@ -573,7 +574,7 @@
         <v>253.6</v>
       </c>
       <c r="F3" s="2">
-        <v>0</v>
+        <v>194.4</v>
       </c>
       <c r="G3" s="2">
         <v>0</v>
@@ -593,7 +594,7 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B4" s="2">
         <v>132.5</v>
@@ -608,7 +609,7 @@
         <v>48.4</v>
       </c>
       <c r="F4" s="2">
-        <v>0</v>
+        <v>165.6</v>
       </c>
       <c r="G4" s="2">
         <v>0</v>
@@ -628,7 +629,7 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B5" s="2">
         <v>107.5</v>
@@ -643,7 +644,7 @@
         <v>178.8</v>
       </c>
       <c r="F5" s="2">
-        <v>0</v>
+        <v>77.2</v>
       </c>
       <c r="G5" s="2">
         <v>0</v>
@@ -663,7 +664,7 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B6" s="2">
         <v>307.60000000000002</v>
@@ -678,7 +679,7 @@
         <v>288.8</v>
       </c>
       <c r="F6" s="2">
-        <v>0</v>
+        <v>203.5</v>
       </c>
       <c r="G6" s="2">
         <v>0</v>
@@ -698,7 +699,7 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B7" s="2">
         <v>370.6</v>
@@ -713,7 +714,7 @@
         <v>284.39999999999998</v>
       </c>
       <c r="F7" s="2">
-        <v>0</v>
+        <v>212</v>
       </c>
       <c r="G7" s="2">
         <v>0</v>
@@ -733,7 +734,7 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B8" s="2">
         <v>25</v>
@@ -748,7 +749,7 @@
         <v>126.3</v>
       </c>
       <c r="F8" s="2">
-        <v>0</v>
+        <v>201.1</v>
       </c>
       <c r="G8" s="2">
         <v>0</v>
@@ -768,7 +769,7 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B9" s="2">
         <v>31</v>
@@ -783,7 +784,7 @@
         <v>194.2</v>
       </c>
       <c r="F9" s="2">
-        <v>0</v>
+        <v>72.599999999999994</v>
       </c>
       <c r="G9" s="2">
         <v>0</v>
@@ -803,7 +804,7 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B10" s="2">
         <v>0</v>
@@ -818,7 +819,7 @@
         <v>25</v>
       </c>
       <c r="F10" s="2">
-        <v>0</v>
+        <v>62</v>
       </c>
       <c r="G10" s="2">
         <v>0</v>
@@ -838,7 +839,7 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B11" s="2">
         <v>497.4</v>
@@ -854,7 +855,7 @@
         <v>126.9</v>
       </c>
       <c r="F11" s="2">
-        <v>0</v>
+        <v>266.3</v>
       </c>
       <c r="G11" s="2">
         <v>0</v>
@@ -871,6 +872,33 @@
       <c r="K11" s="2">
         <v>0</v>
       </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B13" s="2"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B14" s="2"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B15" s="2"/>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B18" s="2"/>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B19" s="2"/>
+    </row>
+    <row r="23" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B23" s="2"/>
+    </row>
+    <row r="24" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B24" s="2"/>
+    </row>
+    <row r="27" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B27" s="2"/>
+    </row>
+    <row r="30" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B30" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
latest. updated week 6
</commit_message>
<xml_diff>
--- a/Master_comp.xlsx
+++ b/Master_comp.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\612721\1_Projects\Bourbon_Chasers_MASTER\Bourbon_Chasers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E86B887D-E233-4D2B-90BE-7E5B8B0155E8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B9DD6DA-EA38-4280-B68C-C8B1F8ABCCC5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{1EF4F618-38B6-4D40-964A-FE6EA7248209}"/>
   </bookViews>
@@ -16,7 +16,6 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -42,9 +41,6 @@
     <t>Week 1 -- May 1 - 8</t>
   </si>
   <si>
-    <t>Week 6</t>
-  </si>
-  <si>
     <t>Week 7</t>
   </si>
   <si>
@@ -97,6 +93,9 @@
   </si>
   <si>
     <t>Week 5 -- May 30 - June 5</t>
+  </si>
+  <si>
+    <t>Week 6 -- June 6 - 12</t>
   </si>
 </sst>
 </file>
@@ -470,10 +469,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0652209-7C2F-4DC6-AE94-2767734CF0E0}">
-  <dimension ref="A1:K11"/>
+  <dimension ref="A1:K33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12:XFD1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -483,7 +482,8 @@
     <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="19" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="22.36328125" bestFit="1" customWidth="1"/>
-    <col min="7" max="10" width="7" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.1796875" bestFit="1" customWidth="1"/>
+    <col min="8" max="10" width="7" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -495,36 +495,36 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>5</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B2" s="2">
         <v>193.1</v>
@@ -542,7 +542,7 @@
         <v>38.6</v>
       </c>
       <c r="G2" s="2">
-        <v>0</v>
+        <v>455.4</v>
       </c>
       <c r="H2" s="2">
         <v>0</v>
@@ -559,7 +559,7 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B3">
         <v>253.6</v>
@@ -577,7 +577,7 @@
         <v>194.4</v>
       </c>
       <c r="G3" s="2">
-        <v>0</v>
+        <v>238.6</v>
       </c>
       <c r="H3" s="2">
         <v>0</v>
@@ -594,7 +594,7 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B4" s="2">
         <v>132.5</v>
@@ -612,7 +612,7 @@
         <v>165.6</v>
       </c>
       <c r="G4" s="2">
-        <v>0</v>
+        <v>337.2</v>
       </c>
       <c r="H4" s="2">
         <v>0</v>
@@ -629,7 +629,7 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B5" s="2">
         <v>107.5</v>
@@ -647,7 +647,7 @@
         <v>77.2</v>
       </c>
       <c r="G5" s="2">
-        <v>0</v>
+        <v>43.3</v>
       </c>
       <c r="H5" s="2">
         <v>0</v>
@@ -664,7 +664,7 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B6" s="2">
         <v>307.60000000000002</v>
@@ -682,7 +682,7 @@
         <v>203.5</v>
       </c>
       <c r="G6" s="2">
-        <v>0</v>
+        <v>388.1</v>
       </c>
       <c r="H6" s="2">
         <v>0</v>
@@ -699,7 +699,7 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B7" s="2">
         <v>370.6</v>
@@ -717,7 +717,7 @@
         <v>212</v>
       </c>
       <c r="G7" s="2">
-        <v>0</v>
+        <v>243.2</v>
       </c>
       <c r="H7" s="2">
         <v>0</v>
@@ -734,7 +734,7 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B8" s="2">
         <v>25</v>
@@ -752,7 +752,7 @@
         <v>201.1</v>
       </c>
       <c r="G8" s="2">
-        <v>0</v>
+        <v>169.7</v>
       </c>
       <c r="H8" s="2">
         <v>0</v>
@@ -769,7 +769,7 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B9" s="2">
         <v>31</v>
@@ -804,7 +804,7 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B10" s="2">
         <v>0</v>
@@ -822,7 +822,7 @@
         <v>62</v>
       </c>
       <c r="G10" s="2">
-        <v>0</v>
+        <v>41</v>
       </c>
       <c r="H10" s="2">
         <v>0</v>
@@ -839,7 +839,7 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B11" s="2">
         <v>497.4</v>
@@ -858,7 +858,7 @@
         <v>266.3</v>
       </c>
       <c r="G11" s="2">
-        <v>0</v>
+        <v>373.4</v>
       </c>
       <c r="H11" s="2">
         <v>0</v>
@@ -872,6 +872,42 @@
       <c r="K11" s="2">
         <v>0</v>
       </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B13" s="2"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B14" s="2"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B15" s="2"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B16" s="2"/>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B17" s="2"/>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B18" s="2"/>
+    </row>
+    <row r="21" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B21" s="2"/>
+    </row>
+    <row r="22" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B22" s="2"/>
+    </row>
+    <row r="27" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B27" s="2"/>
+    </row>
+    <row r="29" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B29" s="2"/>
+    </row>
+    <row r="31" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B31" s="2"/>
+    </row>
+    <row r="33" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B33" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
latest. update the weekly points
</commit_message>
<xml_diff>
--- a/Master_comp.xlsx
+++ b/Master_comp.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\612721\1_Projects\Bourbon_Chasers_MASTER\Bourbon_Chasers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B9DD6DA-EA38-4280-B68C-C8B1F8ABCCC5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E51C5248-A25D-4DF2-984F-138E2B7F5B3F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{1EF4F618-38B6-4D40-964A-FE6EA7248209}"/>
   </bookViews>
@@ -41,9 +41,6 @@
     <t>Week 1 -- May 1 - 8</t>
   </si>
   <si>
-    <t>Week 7</t>
-  </si>
-  <si>
     <t>Week 8</t>
   </si>
   <si>
@@ -96,6 +93,9 @@
   </si>
   <si>
     <t>Week 6 -- June 6 - 12</t>
+  </si>
+  <si>
+    <t>Week 7 -- June 13 - 19</t>
   </si>
 </sst>
 </file>
@@ -469,10 +469,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0652209-7C2F-4DC6-AE94-2767734CF0E0}">
-  <dimension ref="A1:K33"/>
+  <dimension ref="A1:K37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -483,7 +483,8 @@
     <col min="4" max="5" width="19" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="22.36328125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="18.1796875" bestFit="1" customWidth="1"/>
-    <col min="8" max="10" width="7" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.1796875" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="7" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -495,36 +496,36 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>4</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B2" s="2">
         <v>193.1</v>
@@ -545,7 +546,7 @@
         <v>455.4</v>
       </c>
       <c r="H2" s="2">
-        <v>0</v>
+        <v>306.10000000000002</v>
       </c>
       <c r="I2" s="2">
         <v>0</v>
@@ -559,7 +560,7 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B3">
         <v>253.6</v>
@@ -580,7 +581,7 @@
         <v>238.6</v>
       </c>
       <c r="H3" s="2">
-        <v>0</v>
+        <v>203.1</v>
       </c>
       <c r="I3" s="2">
         <v>0</v>
@@ -594,7 +595,7 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B4" s="2">
         <v>132.5</v>
@@ -615,7 +616,7 @@
         <v>337.2</v>
       </c>
       <c r="H4" s="2">
-        <v>0</v>
+        <v>216.1</v>
       </c>
       <c r="I4" s="2">
         <v>0</v>
@@ -629,7 +630,7 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B5" s="2">
         <v>107.5</v>
@@ -650,7 +651,7 @@
         <v>43.3</v>
       </c>
       <c r="H5" s="2">
-        <v>0</v>
+        <v>208.2</v>
       </c>
       <c r="I5" s="2">
         <v>0</v>
@@ -664,7 +665,7 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B6" s="2">
         <v>307.60000000000002</v>
@@ -685,7 +686,7 @@
         <v>388.1</v>
       </c>
       <c r="H6" s="2">
-        <v>0</v>
+        <v>269.60000000000002</v>
       </c>
       <c r="I6" s="2">
         <v>0</v>
@@ -699,7 +700,7 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B7" s="2">
         <v>370.6</v>
@@ -720,7 +721,7 @@
         <v>243.2</v>
       </c>
       <c r="H7" s="2">
-        <v>0</v>
+        <v>480</v>
       </c>
       <c r="I7" s="2">
         <v>0</v>
@@ -734,7 +735,7 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B8" s="2">
         <v>25</v>
@@ -755,7 +756,7 @@
         <v>169.7</v>
       </c>
       <c r="H8" s="2">
-        <v>0</v>
+        <v>189.6</v>
       </c>
       <c r="I8" s="2">
         <v>0</v>
@@ -769,7 +770,7 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B9" s="2">
         <v>31</v>
@@ -804,7 +805,7 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B10" s="2">
         <v>0</v>
@@ -839,7 +840,7 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B11" s="2">
         <v>497.4</v>
@@ -861,7 +862,7 @@
         <v>373.4</v>
       </c>
       <c r="H11" s="2">
-        <v>0</v>
+        <v>429</v>
       </c>
       <c r="I11" s="2">
         <v>0</v>
@@ -897,17 +898,26 @@
     <row r="22" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B22" s="2"/>
     </row>
+    <row r="23" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B23" s="2"/>
+    </row>
     <row r="27" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B27" s="2"/>
     </row>
     <row r="29" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B29" s="2"/>
     </row>
+    <row r="30" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B30" s="2"/>
+    </row>
     <row r="31" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B31" s="2"/>
     </row>
     <row r="33" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B33" s="2"/>
+    </row>
+    <row r="37" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B37" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
latest. Updated wk 8
</commit_message>
<xml_diff>
--- a/Master_comp.xlsx
+++ b/Master_comp.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\612721\1_Projects\Bourbon_Chasers_MASTER\Bourbon_Chasers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E51C5248-A25D-4DF2-984F-138E2B7F5B3F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E2B5D1D-333E-4B6F-A09C-065EAF42B427}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{1EF4F618-38B6-4D40-964A-FE6EA7248209}"/>
+    <workbookView minimized="1" xWindow="2370" yWindow="0" windowWidth="14400" windowHeight="10200" xr2:uid="{1EF4F618-38B6-4D40-964A-FE6EA7248209}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -41,9 +41,6 @@
     <t>Week 1 -- May 1 - 8</t>
   </si>
   <si>
-    <t>Week 8</t>
-  </si>
-  <si>
     <t>Week 9</t>
   </si>
   <si>
@@ -96,6 +93,9 @@
   </si>
   <si>
     <t>Week 7 -- June 13 - 19</t>
+  </si>
+  <si>
+    <t>Week 8 -- June 20 - 26</t>
   </si>
 </sst>
 </file>
@@ -472,7 +472,7 @@
   <dimension ref="A1:K37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -483,8 +483,8 @@
     <col min="4" max="5" width="19" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="22.36328125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="18.1796875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.1796875" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="7" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="19.1796875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -496,36 +496,36 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B2" s="2">
         <v>193.1</v>
@@ -549,7 +549,7 @@
         <v>306.10000000000002</v>
       </c>
       <c r="I2" s="2">
-        <v>0</v>
+        <v>224.7</v>
       </c>
       <c r="J2" s="2">
         <v>0</v>
@@ -560,7 +560,7 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B3">
         <v>253.6</v>
@@ -584,7 +584,7 @@
         <v>203.1</v>
       </c>
       <c r="I3" s="2">
-        <v>0</v>
+        <v>223.2</v>
       </c>
       <c r="J3" s="2">
         <v>0</v>
@@ -595,7 +595,7 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B4" s="2">
         <v>132.5</v>
@@ -619,7 +619,7 @@
         <v>216.1</v>
       </c>
       <c r="I4" s="2">
-        <v>0</v>
+        <v>104</v>
       </c>
       <c r="J4" s="2">
         <v>0</v>
@@ -630,7 +630,7 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B5" s="2">
         <v>107.5</v>
@@ -654,7 +654,7 @@
         <v>208.2</v>
       </c>
       <c r="I5" s="2">
-        <v>0</v>
+        <v>123.6</v>
       </c>
       <c r="J5" s="2">
         <v>0</v>
@@ -665,7 +665,7 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B6" s="2">
         <v>307.60000000000002</v>
@@ -689,7 +689,7 @@
         <v>269.60000000000002</v>
       </c>
       <c r="I6" s="2">
-        <v>0</v>
+        <v>402.1</v>
       </c>
       <c r="J6" s="2">
         <v>0</v>
@@ -700,7 +700,7 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B7" s="2">
         <v>370.6</v>
@@ -724,7 +724,7 @@
         <v>480</v>
       </c>
       <c r="I7" s="2">
-        <v>0</v>
+        <v>309.7</v>
       </c>
       <c r="J7" s="2">
         <v>0</v>
@@ -735,7 +735,7 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B8" s="2">
         <v>25</v>
@@ -759,7 +759,7 @@
         <v>189.6</v>
       </c>
       <c r="I8" s="2">
-        <v>0</v>
+        <v>51.2</v>
       </c>
       <c r="J8" s="2">
         <v>0</v>
@@ -770,7 +770,7 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B9" s="2">
         <v>31</v>
@@ -794,7 +794,7 @@
         <v>0</v>
       </c>
       <c r="I9" s="2">
-        <v>0</v>
+        <v>269.89999999999998</v>
       </c>
       <c r="J9" s="2">
         <v>0</v>
@@ -805,7 +805,7 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B10" s="2">
         <v>0</v>
@@ -840,7 +840,7 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B11" s="2">
         <v>497.4</v>
@@ -865,7 +865,7 @@
         <v>429</v>
       </c>
       <c r="I11" s="2">
-        <v>0</v>
+        <v>352.4</v>
       </c>
       <c r="J11" s="2">
         <v>0</v>
@@ -892,6 +892,9 @@
     <row r="18" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B18" s="2"/>
     </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B19" s="2"/>
+    </row>
     <row r="21" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B21" s="2"/>
     </row>
@@ -901,6 +904,15 @@
     <row r="23" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B23" s="2"/>
     </row>
+    <row r="24" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B24" s="2"/>
+    </row>
+    <row r="25" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B25" s="2"/>
+    </row>
+    <row r="26" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B26" s="2"/>
+    </row>
     <row r="27" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B27" s="2"/>
     </row>
@@ -915,6 +927,9 @@
     </row>
     <row r="33" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B33" s="2"/>
+    </row>
+    <row r="36" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B36" s="2"/>
     </row>
     <row r="37" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B37" s="2"/>

</xml_diff>

<commit_message>
latest. Updated wk 9
</commit_message>
<xml_diff>
--- a/Master_comp.xlsx
+++ b/Master_comp.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\612721\1_Projects\Bourbon_Chasers_MASTER\Bourbon_Chasers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E2B5D1D-333E-4B6F-A09C-065EAF42B427}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2486082-DB38-4E1A-8ED2-8A9A1BE95FA2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="2370" yWindow="0" windowWidth="14400" windowHeight="10200" xr2:uid="{1EF4F618-38B6-4D40-964A-FE6EA7248209}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{1EF4F618-38B6-4D40-964A-FE6EA7248209}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -41,9 +41,6 @@
     <t>Week 1 -- May 1 - 8</t>
   </si>
   <si>
-    <t>Week 9</t>
-  </si>
-  <si>
     <t>Week 10</t>
   </si>
   <si>
@@ -96,6 +93,9 @@
   </si>
   <si>
     <t>Week 8 -- June 20 - 26</t>
+  </si>
+  <si>
+    <t>Week 9 -- June27 - July 3</t>
   </si>
 </sst>
 </file>
@@ -471,8 +471,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0652209-7C2F-4DC6-AE94-2767734CF0E0}">
   <dimension ref="A1:K37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -484,7 +484,7 @@
     <col min="6" max="6" width="22.36328125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="18.1796875" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="19.1796875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="21.36328125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -496,36 +496,36 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>2</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B2" s="2">
         <v>193.1</v>
@@ -552,7 +552,7 @@
         <v>224.7</v>
       </c>
       <c r="J2" s="2">
-        <v>0</v>
+        <v>141.1</v>
       </c>
       <c r="K2" s="2">
         <v>0</v>
@@ -560,7 +560,7 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B3">
         <v>253.6</v>
@@ -587,7 +587,7 @@
         <v>223.2</v>
       </c>
       <c r="J3" s="2">
-        <v>0</v>
+        <v>83.8</v>
       </c>
       <c r="K3" s="2">
         <v>0</v>
@@ -595,7 +595,7 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B4" s="2">
         <v>132.5</v>
@@ -622,7 +622,7 @@
         <v>104</v>
       </c>
       <c r="J4" s="2">
-        <v>0</v>
+        <v>79.2</v>
       </c>
       <c r="K4" s="2">
         <v>0</v>
@@ -630,7 +630,7 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B5" s="2">
         <v>107.5</v>
@@ -657,7 +657,7 @@
         <v>123.6</v>
       </c>
       <c r="J5" s="2">
-        <v>0</v>
+        <v>274.89999999999998</v>
       </c>
       <c r="K5" s="2">
         <v>0</v>
@@ -665,7 +665,7 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B6" s="2">
         <v>307.60000000000002</v>
@@ -692,7 +692,7 @@
         <v>402.1</v>
       </c>
       <c r="J6" s="2">
-        <v>0</v>
+        <v>321.5</v>
       </c>
       <c r="K6" s="2">
         <v>0</v>
@@ -700,7 +700,7 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B7" s="2">
         <v>370.6</v>
@@ -727,7 +727,7 @@
         <v>309.7</v>
       </c>
       <c r="J7" s="2">
-        <v>0</v>
+        <v>104.9</v>
       </c>
       <c r="K7" s="2">
         <v>0</v>
@@ -735,7 +735,7 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B8" s="2">
         <v>25</v>
@@ -762,7 +762,7 @@
         <v>51.2</v>
       </c>
       <c r="J8" s="2">
-        <v>0</v>
+        <v>65.900000000000006</v>
       </c>
       <c r="K8" s="2">
         <v>0</v>
@@ -770,7 +770,7 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B9" s="2">
         <v>31</v>
@@ -797,7 +797,7 @@
         <v>269.89999999999998</v>
       </c>
       <c r="J9" s="2">
-        <v>0</v>
+        <v>88</v>
       </c>
       <c r="K9" s="2">
         <v>0</v>
@@ -805,7 +805,7 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B10" s="2">
         <v>0</v>
@@ -840,7 +840,7 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B11" s="2">
         <v>497.4</v>
@@ -868,7 +868,7 @@
         <v>352.4</v>
       </c>
       <c r="J11" s="2">
-        <v>0</v>
+        <v>173.7</v>
       </c>
       <c r="K11" s="2">
         <v>0</v>
@@ -876,62 +876,69 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B13" s="2"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B14" s="2"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B15" s="2"/>
+      <c r="I15" s="2"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B16" s="2"/>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B17" s="2"/>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B18" s="2"/>
     </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B19" s="2"/>
-    </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="I19" s="2"/>
+    </row>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B21" s="2"/>
     </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B22" s="2"/>
     </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B23" s="2"/>
-    </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="H23" s="2"/>
+      <c r="I23" s="2"/>
+    </row>
+    <row r="24" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B24" s="2"/>
     </row>
-    <row r="25" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B25" s="2"/>
     </row>
-    <row r="26" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B26" s="2"/>
     </row>
-    <row r="27" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B27" s="2"/>
     </row>
-    <row r="29" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B29" s="2"/>
     </row>
-    <row r="30" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B30" s="2"/>
     </row>
-    <row r="31" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B31" s="2"/>
     </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B33" s="2"/>
-    </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="I33" s="2"/>
+    </row>
+    <row r="36" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B36" s="2"/>
     </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="37" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B37" s="2"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
latest. Updated wk 10
</commit_message>
<xml_diff>
--- a/Master_comp.xlsx
+++ b/Master_comp.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\612721\1_Projects\Bourbon_Chasers_MASTER\Bourbon_Chasers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2486082-DB38-4E1A-8ED2-8A9A1BE95FA2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3ED2297-8857-49B2-8864-A1F45AFD4D8F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{1EF4F618-38B6-4D40-964A-FE6EA7248209}"/>
   </bookViews>
@@ -41,9 +41,6 @@
     <t>Week 1 -- May 1 - 8</t>
   </si>
   <si>
-    <t>Week 10</t>
-  </si>
-  <si>
     <t>Jeremiah Gaddy</t>
   </si>
   <si>
@@ -96,6 +93,9 @@
   </si>
   <si>
     <t>Week 9 -- June27 - July 3</t>
+  </si>
+  <si>
+    <t>Week 10 -- July 4 - 10</t>
   </si>
 </sst>
 </file>
@@ -471,8 +471,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0652209-7C2F-4DC6-AE94-2767734CF0E0}">
   <dimension ref="A1:K37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -485,7 +485,7 @@
     <col min="7" max="7" width="18.1796875" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="19.1796875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="21.36328125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.35">
@@ -496,36 +496,36 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B2" s="2">
         <v>193.1</v>
@@ -555,12 +555,12 @@
         <v>141.1</v>
       </c>
       <c r="K2" s="2">
-        <v>0</v>
+        <v>255.2</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B3">
         <v>253.6</v>
@@ -590,12 +590,12 @@
         <v>83.8</v>
       </c>
       <c r="K3" s="2">
-        <v>0</v>
+        <v>38.700000000000003</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B4" s="2">
         <v>132.5</v>
@@ -625,12 +625,12 @@
         <v>79.2</v>
       </c>
       <c r="K4" s="2">
-        <v>0</v>
+        <v>117.4</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B5" s="2">
         <v>107.5</v>
@@ -660,12 +660,12 @@
         <v>274.89999999999998</v>
       </c>
       <c r="K5" s="2">
-        <v>0</v>
+        <v>139.5</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B6" s="2">
         <v>307.60000000000002</v>
@@ -695,12 +695,12 @@
         <v>321.5</v>
       </c>
       <c r="K6" s="2">
-        <v>0</v>
+        <v>322.39999999999998</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B7" s="2">
         <v>370.6</v>
@@ -730,12 +730,12 @@
         <v>104.9</v>
       </c>
       <c r="K7" s="2">
-        <v>0</v>
+        <v>95.9</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B8" s="2">
         <v>25</v>
@@ -765,12 +765,12 @@
         <v>65.900000000000006</v>
       </c>
       <c r="K8" s="2">
-        <v>0</v>
+        <v>212.7</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B9" s="2">
         <v>31</v>
@@ -805,7 +805,7 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B10" s="2">
         <v>0</v>
@@ -840,7 +840,7 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B11" s="2">
         <v>497.4</v>
@@ -871,74 +871,97 @@
         <v>173.7</v>
       </c>
       <c r="K11" s="2">
-        <v>0</v>
+        <v>458.2</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B13" s="2"/>
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
+      <c r="J13" s="2"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B14" s="2"/>
+      <c r="J14" s="2"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B15" s="2"/>
       <c r="I15" s="2"/>
+      <c r="J15" s="2"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B16" s="2"/>
-    </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="J16" s="2"/>
+    </row>
+    <row r="17" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B17" s="2"/>
-    </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="J17" s="2"/>
+    </row>
+    <row r="18" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B18" s="2"/>
-    </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="J18" s="2"/>
+    </row>
+    <row r="19" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B19" s="2"/>
       <c r="I19" s="2"/>
-    </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="J19" s="2"/>
+    </row>
+    <row r="20" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="J20" s="2"/>
+    </row>
+    <row r="21" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B21" s="2"/>
-    </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="J21" s="2"/>
+    </row>
+    <row r="22" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B22" s="2"/>
-    </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="J22" s="2"/>
+    </row>
+    <row r="23" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B23" s="2"/>
       <c r="H23" s="2"/>
       <c r="I23" s="2"/>
-    </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="J23" s="2"/>
+    </row>
+    <row r="24" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B24" s="2"/>
     </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B25" s="2"/>
     </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B26" s="2"/>
-    </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="J26" s="2"/>
+    </row>
+    <row r="27" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B27" s="2"/>
-    </row>
-    <row r="29" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="J27" s="2"/>
+    </row>
+    <row r="28" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="I28" s="2"/>
+    </row>
+    <row r="29" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B29" s="2"/>
-    </row>
-    <row r="30" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="J29" s="2"/>
+    </row>
+    <row r="30" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B30" s="2"/>
-    </row>
-    <row r="31" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="J30" s="2"/>
+    </row>
+    <row r="31" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B31" s="2"/>
     </row>
-    <row r="33" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B33" s="2"/>
       <c r="I33" s="2"/>
     </row>
-    <row r="36" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="35" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="J35" s="2"/>
+    </row>
+    <row r="36" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B36" s="2"/>
     </row>
-    <row r="37" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="37" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B37" s="2"/>
     </row>
   </sheetData>

</xml_diff>